<commit_message>
add codes and data
</commit_message>
<xml_diff>
--- a/data/variables.xlsx
+++ b/data/variables.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wodediannao/Desktop/da2-assignment2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DBD598D-0F51-9C41-8392-B1D3A8A1ADB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB93AC8D-4977-1944-B13D-4403DE6D1AFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="60" windowWidth="28040" windowHeight="17440" xr2:uid="{0CC01ACC-52B0-FB43-81EA-88F75F4AA985}"/>
+    <workbookView xWindow="7880" yWindow="720" windowWidth="28040" windowHeight="17440" xr2:uid="{0CC01ACC-52B0-FB43-81EA-88F75F4AA985}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="ConceptsClassifications" localSheetId="0">Sheet1!$D$4</definedName>
+    <definedName name="DataCharacteristics" localSheetId="0">Sheet1!$D$2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,9 +38,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>xx</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">variables </t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>decription</t>
+  </si>
+  <si>
+    <t>Employment Rate</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>Percentage of the working-age population (aged 15-64)</t>
+  </si>
+  <si>
+    <t>Air pollution</t>
+  </si>
+  <si>
+    <t>Micrograms per cubic metre</t>
+  </si>
+  <si>
+    <t>The indicator is the population weighted average of annual concentrations of particulate matters less than 2.5 microns in diameter (PM2.5) in the air. Data are averaged over a three-year period.</t>
+  </si>
+  <si>
+    <t>Water quality</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>The indicator captures people's subjective appreciation of the environment where they live, in particular the quality of the water. It is based on the question: "In the city or area where you live, are you satisfied or dissatisfied with the quality of water?" and it considers people who responded they are satisfied.</t>
+  </si>
+  <si>
+    <t>Quality of support network</t>
+  </si>
+  <si>
+    <t>It's a measure of perceived social network support. The indicator is based on the question: “If you were in trouble, do you have relatives or friends you can count on to help you whenever you need them, or not?” and it considers the respondents who respond positively.
+“High”/ “Low” refer to the percentage of people with tertiary/ below upper secondary education.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Voter turnout</t>
+  </si>
+  <si>
+    <t>Voter turnout is here defined as the ratio between the number of individuals that cast a ballot during an election (whether this vote is valid or not) to the population registered to vote. As institutional features of voting systems vary a lot across countries and across types of elections, the indicator refers to the elections (parliamentary or presidential) that have attracted the largest number of voters in each country.</t>
+  </si>
+  <si>
+    <t>Life expectancy measures how long on average people could expect to live based on the age-specific death rates currently prevailing. This measure refers to people born today and is computed as a weighted average of life expectancy for men and women.</t>
+  </si>
+  <si>
+    <t>Life Expectancy</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>The indicator is based on the question: "Do you feel safe walking alone at night in the city or area where you live?" and it shows people declaring they feel safe.</t>
+  </si>
+  <si>
+    <t>Feeling safe walking alone at night</t>
+  </si>
+  <si>
+    <t>Deaths due to assault</t>
+  </si>
+  <si>
+    <t>Homicide rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Life satisfaction</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>The indicator considers people's evaluation of their life as a whole. It is a weighted-sum of different response categories based on people's rates of their current life relative to the best and worst possible lives for them on a scale from 0 to 10, using the Cantril Ladder (known also as the "Self-Anchoring Striving Scale").
+“High”/ “Low” refer to values for people with tertiary/ below upper secondary education.</t>
   </si>
 </sst>
 </file>
@@ -72,8 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,17 +478,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8B5275-69F3-3D46-BAC5-0759E0188D79}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="97" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>